<commit_message>
working 0.6 firmware: new RAM implementation
</commit_message>
<xml_diff>
--- a/doc/flower-register-map.xlsx
+++ b/doc/flower-register-map.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erico\Desktop\projects\greenland_lowthreshold_system\FLOWER-board-firmware\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\projects\FLOWER-board-firmware\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81E594C-3C44-4BC9-8448-1DF84030EC84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="2115" yWindow="600" windowWidth="23235" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="201">
   <si>
     <t>Register Map</t>
   </si>
@@ -553,15 +555,9 @@
     <t>lower four bits clear each of the 4 event buffers, bit 8 sets buffer to 0, bit 16 is buffer clear for surface event buffer</t>
   </si>
   <si>
-    <t>lower three bits used, set value to 0 thru 7. Pretrig window set to value*8*10.66ns. Middle byte for surface array</t>
-  </si>
-  <si>
     <t>x000404</t>
   </si>
   <si>
-    <t>Default updated 9/1/2017 and tested: puts triggered pulse at beginning of readout window. Surface stuff added 1/15/2019</t>
-  </si>
-  <si>
     <t>bits 3 to 0-&gt;buffer full flags; bit 4-&gt;surface buffer full (slave board only); bit 8-&gt;OR of buffer full flags; bits 13 to 12-&gt;next_buffer ; bits 17 to 16-&gt; last trig type</t>
   </si>
   <si>
@@ -638,13 +634,16 @@
   </si>
   <si>
     <t>lowest byte : num_coinc (0 = 1 ch); middle byte : coinc_window; high byte (LSB = 1 vpp mode; =0 single-side Vp mode)</t>
+  </si>
+  <si>
+    <t>lower three bits used, set value to 0 thru 7.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,6 +704,13 @@
     <font>
       <sz val="11"/>
       <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -810,7 +816,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -897,11 +903,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1183,57 +1196,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="4" width="87.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="6" max="6" width="74.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="4" width="87.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="74.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
-        <v>177</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="47">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="49">
         <v>44212</v>
       </c>
-      <c r="B4" s="48"/>
+      <c r="B4" s="50"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>37</v>
@@ -1242,13 +1255,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1267,7 +1280,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1283,7 +1296,7 @@
       </c>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1298,7 +1311,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>1+A8</f>
         <v>2</v>
@@ -1314,7 +1327,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ref="A10:A73" si="1">1+A9</f>
         <v>3</v>
@@ -1333,7 +1346,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1352,7 +1365,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1371,7 +1384,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1390,7 +1403,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1406,10 +1419,10 @@
         <v>16</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1428,7 +1441,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1444,7 +1457,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1466,7 +1479,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1486,7 +1499,7 @@
       </c>
       <c r="F18" s="19"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1506,7 +1519,7 @@
       </c>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1526,7 +1539,7 @@
       </c>
       <c r="F20" s="19"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1546,7 +1559,7 @@
       </c>
       <c r="F21" s="19"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1566,7 +1579,7 @@
       </c>
       <c r="F22" s="19"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1588,7 +1601,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1610,7 +1623,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1632,7 +1645,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1652,7 +1665,7 @@
       </c>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1672,7 +1685,7 @@
       </c>
       <c r="F27" s="19"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1692,7 +1705,7 @@
       </c>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1712,7 +1725,7 @@
       </c>
       <c r="F29" s="19"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1732,7 +1745,7 @@
       </c>
       <c r="F30" s="19"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1752,7 +1765,7 @@
       </c>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1772,7 +1785,7 @@
       </c>
       <c r="F32" s="19"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1792,7 +1805,7 @@
       </c>
       <c r="F33" s="19"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1812,7 +1825,7 @@
       </c>
       <c r="F34" s="19"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1832,7 +1845,7 @@
       </c>
       <c r="F35" s="19"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -1852,7 +1865,7 @@
       </c>
       <c r="F36" s="19"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -1872,7 +1885,7 @@
       </c>
       <c r="F37" s="19"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -1892,7 +1905,7 @@
       </c>
       <c r="F38" s="19"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -1912,7 +1925,7 @@
       </c>
       <c r="F39" s="19"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -1932,7 +1945,7 @@
       </c>
       <c r="F40" s="19"/>
     </row>
-    <row r="41" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -1942,13 +1955,13 @@
         <v>x22</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D41" s="43"/>
       <c r="E41" s="43"/>
       <c r="F41" s="44"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -1967,7 +1980,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -1986,7 +1999,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -2005,7 +2018,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -2024,7 +2037,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2046,7 +2059,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2065,7 +2078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -2087,7 +2100,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -2100,7 +2113,7 @@
         <v>29</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E49" t="s">
         <v>6</v>
@@ -2109,7 +2122,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2119,7 +2132,7 @@
         <v>x2B</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -2138,7 +2151,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -2157,7 +2170,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -2167,7 +2180,7 @@
         <v>x2E</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -2178,7 +2191,7 @@
       </c>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -2200,7 +2213,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -2210,7 +2223,7 @@
         <v>x31</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -2220,7 +2233,7 @@
         <v>x32</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -2230,7 +2243,7 @@
         <v>x33</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -2240,7 +2253,7 @@
         <v>x34</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -2250,7 +2263,7 @@
         <v>x35</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -2260,7 +2273,7 @@
         <v>x36</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -2270,7 +2283,7 @@
         <v>x37</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2283,16 +2296,16 @@
         <v>21</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -2305,16 +2318,16 @@
         <v>22</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -2324,16 +2337,16 @@
         <v>x3A</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E65" s="34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -2343,16 +2356,16 @@
         <v>x3B</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E66" s="34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -2362,16 +2375,16 @@
         <v>x3C</v>
       </c>
       <c r="C67" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E67" s="34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -2387,7 +2400,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -2406,7 +2419,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -2422,7 +2435,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -2441,7 +2454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -2460,7 +2473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -2470,13 +2483,13 @@
         <v>x42</v>
       </c>
       <c r="C73" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <f t="shared" ref="A74:A134" si="3">1+A73</f>
         <v>67</v>
@@ -2487,7 +2500,7 @@
       </c>
       <c r="F74" s="10"/>
     </row>
-    <row r="75" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <f t="shared" si="3"/>
         <v>68</v>
@@ -2498,7 +2511,7 @@
       </c>
       <c r="F75" s="10"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <f t="shared" si="3"/>
         <v>69</v>
@@ -2520,7 +2533,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <f t="shared" si="3"/>
         <v>70</v>
@@ -2531,7 +2544,7 @@
       </c>
       <c r="F77" s="10"/>
     </row>
-    <row r="78" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <f t="shared" si="3"/>
         <v>71</v>
@@ -2553,7 +2566,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <f t="shared" si="3"/>
         <v>72</v>
@@ -2575,7 +2588,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <f t="shared" si="3"/>
         <v>73</v>
@@ -2586,7 +2599,7 @@
       </c>
       <c r="E80" s="4"/>
     </row>
-    <row r="81" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <f t="shared" si="3"/>
         <v>74</v>
@@ -2599,7 +2612,7 @@
       <c r="D81" s="12"/>
       <c r="F81" s="10"/>
     </row>
-    <row r="82" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <f t="shared" si="3"/>
         <v>75</v>
@@ -2621,7 +2634,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="3"/>
         <v>76</v>
@@ -2634,16 +2647,13 @@
         <v>35</v>
       </c>
       <c r="D83" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E83" t="s">
         <v>173</v>
       </c>
-      <c r="E83" t="s">
-        <v>174</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="3"/>
         <v>77</v>
@@ -2665,7 +2675,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="3"/>
         <v>78</v>
@@ -2687,7 +2697,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="3"/>
         <v>79</v>
@@ -2700,7 +2710,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="3"/>
         <v>80</v>
@@ -2709,20 +2719,20 @@
         <f t="shared" si="2"/>
         <v>x50</v>
       </c>
-      <c r="C87" s="49" t="s">
+      <c r="C87" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="D87" s="50" t="s">
+      <c r="D87" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="E87" s="49" t="s">
+      <c r="E87" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="F87" s="50" t="s">
+      <c r="F87" s="47" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="3"/>
         <v>81</v>
@@ -2731,20 +2741,20 @@
         <f t="shared" si="2"/>
         <v>x51</v>
       </c>
-      <c r="C88" s="49" t="s">
+      <c r="C88" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="D88" s="50" t="s">
+      <c r="D88" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="E88" s="49" t="s">
+      <c r="E88" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="F88" s="50" t="s">
+      <c r="F88" s="47" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="3"/>
         <v>82</v>
@@ -2753,20 +2763,20 @@
         <f t="shared" si="2"/>
         <v>x52</v>
       </c>
-      <c r="C89" s="49" t="s">
+      <c r="C89" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="D89" s="50" t="s">
+      <c r="D89" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="E89" s="49" t="s">
+      <c r="E89" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="F89" s="50" t="s">
+      <c r="F89" s="47" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="3"/>
         <v>83</v>
@@ -2775,20 +2785,20 @@
         <f t="shared" si="2"/>
         <v>x53</v>
       </c>
-      <c r="C90" s="49" t="s">
+      <c r="C90" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="D90" s="50" t="s">
+      <c r="D90" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="E90" s="49" t="s">
+      <c r="E90" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="F90" s="50" t="s">
+      <c r="F90" s="47" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="3"/>
         <v>84</v>
@@ -2797,20 +2807,20 @@
         <f t="shared" si="2"/>
         <v>x54</v>
       </c>
-      <c r="C91" s="49" t="s">
+      <c r="C91" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="D91" s="49" t="s">
+      <c r="D91" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="E91" s="49" t="s">
+      <c r="E91" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="F91" s="50" t="s">
+      <c r="F91" s="47" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="3"/>
         <v>85</v>
@@ -2819,18 +2829,18 @@
         <f t="shared" si="2"/>
         <v>x55</v>
       </c>
-      <c r="C92" s="49" t="s">
+      <c r="C92" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="D92" s="50" t="s">
+      <c r="D92" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="E92" s="49" t="s">
+      <c r="E92" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F92" s="50"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F92" s="47"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="3"/>
         <v>86</v>
@@ -2841,7 +2851,7 @@
       </c>
       <c r="E93" s="11"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="3"/>
         <v>87</v>
@@ -2851,16 +2861,16 @@
         <v>x57</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E94" s="45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="3"/>
         <v>88</v>
@@ -2870,16 +2880,16 @@
         <v>x58</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E95" s="45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="3"/>
         <v>89</v>
@@ -2889,16 +2899,16 @@
         <v>x59</v>
       </c>
       <c r="C96" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="D96" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>197</v>
       </c>
       <c r="E96" s="45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="3"/>
         <v>90</v>
@@ -2908,16 +2918,16 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="45" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E97" s="45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="3"/>
         <v>91</v>
@@ -2927,16 +2937,16 @@
         <v>x5B</v>
       </c>
       <c r="C98" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E98" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="D98" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="E98" s="45" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="3"/>
         <v>92</v>
@@ -2949,7 +2959,7 @@
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="3"/>
         <v>93</v>
@@ -2962,7 +2972,7 @@
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" si="3"/>
         <v>94</v>
@@ -2975,7 +2985,7 @@
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <f t="shared" si="3"/>
         <v>95</v>
@@ -2988,7 +2998,7 @@
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <f t="shared" si="3"/>
         <v>96</v>
@@ -3001,7 +3011,7 @@
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <f t="shared" si="3"/>
         <v>97</v>
@@ -3014,7 +3024,7 @@
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <f t="shared" si="3"/>
         <v>98</v>
@@ -3027,7 +3037,7 @@
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <f t="shared" si="3"/>
         <v>99</v>
@@ -3040,7 +3050,7 @@
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <f t="shared" si="3"/>
         <v>100</v>
@@ -3053,7 +3063,7 @@
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <f t="shared" si="3"/>
         <v>101</v>
@@ -3066,7 +3076,7 @@
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
     </row>
-    <row r="109" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="35">
         <f t="shared" si="3"/>
         <v>102</v>
@@ -3085,7 +3095,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="110" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="31">
         <f t="shared" si="3"/>
         <v>103</v>
@@ -3101,10 +3111,10 @@
         <v>144</v>
       </c>
       <c r="F110" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="31">
         <f t="shared" si="3"/>
         <v>104</v>
@@ -3117,10 +3127,10 @@
         <v>141</v>
       </c>
       <c r="F111" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="31">
         <f t="shared" si="3"/>
         <v>105</v>
@@ -3133,10 +3143,10 @@
         <v>142</v>
       </c>
       <c r="F112" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="31">
         <f t="shared" si="3"/>
         <v>106</v>
@@ -3149,10 +3159,10 @@
         <v>145</v>
       </c>
       <c r="F113" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="31">
         <f t="shared" si="3"/>
         <v>107</v>
@@ -3165,10 +3175,10 @@
         <v>146</v>
       </c>
       <c r="F114" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <f t="shared" si="3"/>
         <v>108</v>
@@ -3190,7 +3200,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <f t="shared" si="3"/>
         <v>109</v>
@@ -3212,7 +3222,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="117" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="31">
         <f t="shared" si="3"/>
         <v>110</v>
@@ -3228,10 +3238,10 @@
         <v>127</v>
       </c>
       <c r="F117" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="31">
         <f t="shared" si="3"/>
         <v>111</v>
@@ -3247,10 +3257,10 @@
         <v>125</v>
       </c>
       <c r="F118" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="31">
         <f t="shared" si="3"/>
         <v>112</v>
@@ -3266,10 +3276,10 @@
         <v>126</v>
       </c>
       <c r="F119" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="31">
         <f t="shared" si="3"/>
         <v>113</v>
@@ -3285,10 +3295,10 @@
         <v>126</v>
       </c>
       <c r="F120" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="31">
         <f t="shared" si="3"/>
         <v>114</v>
@@ -3304,10 +3314,10 @@
         <v>135</v>
       </c>
       <c r="F121" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="31">
         <f t="shared" si="3"/>
         <v>115</v>
@@ -3323,10 +3333,10 @@
         <v>126</v>
       </c>
       <c r="F122" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="31">
         <f t="shared" si="3"/>
         <v>116</v>
@@ -3342,10 +3352,10 @@
         <v>126</v>
       </c>
       <c r="F123" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="31">
         <f t="shared" si="3"/>
         <v>117</v>
@@ -3361,10 +3371,10 @@
         <v>137</v>
       </c>
       <c r="F124" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="31">
         <f t="shared" si="3"/>
         <v>118</v>
@@ -3380,10 +3390,10 @@
         <v>126</v>
       </c>
       <c r="F125" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="31">
         <f t="shared" si="3"/>
         <v>119</v>
@@ -3399,10 +3409,10 @@
         <v>126</v>
       </c>
       <c r="F126" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="31">
         <f t="shared" si="3"/>
         <v>120</v>
@@ -3415,10 +3425,10 @@
         <v>147</v>
       </c>
       <c r="F127" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="31">
         <f t="shared" si="3"/>
         <v>121</v>
@@ -3434,36 +3444,36 @@
         <v>143</v>
       </c>
       <c r="F128" s="33" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <f t="shared" si="3"/>
+        <v>122</v>
+      </c>
+      <c r="B129" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>x7A</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="38">
+        <f t="shared" si="3"/>
+        <v>123</v>
+      </c>
+      <c r="B130" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v>x7B</v>
+      </c>
+      <c r="C130" s="38" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129">
-        <f t="shared" si="3"/>
-        <v>122</v>
-      </c>
-      <c r="B129" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v>x7A</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="38">
-        <f t="shared" si="3"/>
-        <v>123</v>
-      </c>
-      <c r="B130" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v>x7B</v>
-      </c>
-      <c r="C130" s="38" t="s">
-        <v>180</v>
-      </c>
       <c r="F130" s="40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="38">
         <f t="shared" si="3"/>
         <v>124</v>
@@ -3473,13 +3483,13 @@
         <v>x7C</v>
       </c>
       <c r="C131" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="F131" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="F131" s="40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <f t="shared" si="3"/>
         <v>125</v>
@@ -3491,7 +3501,7 @@
       <c r="C132" s="31"/>
       <c r="D132" s="31"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <f t="shared" si="3"/>
         <v>126</v>
@@ -3510,22 +3520,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134">
+    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="51">
         <f t="shared" si="3"/>
         <v>127</v>
       </c>
-      <c r="B134" s="24" t="str">
+      <c r="B134" s="52" t="str">
         <f t="shared" si="2"/>
         <v>x7F</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="D134" s="5" t="s">
+      <c r="D134" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E134" s="51" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add on/off switches for trigger types
</commit_message>
<xml_diff>
--- a/doc/flower-register-map.xlsx
+++ b/doc/flower-register-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\projects\FLOWER-board-firmware\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81E594C-3C44-4BC9-8448-1DF84030EC84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CDD5B5-5C83-4ADA-8082-646D5C6BD07B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="600" windowWidth="23235" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="2205" windowWidth="23235" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="199">
   <si>
     <t>Register Map</t>
   </si>
@@ -537,18 +537,6 @@
     <t>x000C03</t>
   </si>
   <si>
-    <t>trig delay: CH's 0,1,2</t>
-  </si>
-  <si>
-    <t>trig delay: CH's 3,4,5</t>
-  </si>
-  <si>
-    <t>trig delay: CH's 6,7</t>
-  </si>
-  <si>
-    <t>one byte each channel</t>
-  </si>
-  <si>
     <t>note channel 5 hard-coded masked from trigger (dead vpol channel)</t>
   </si>
   <si>
@@ -637,6 +625,12 @@
   </si>
   <si>
     <t>lower three bits used, set value to 0 thru 7.</t>
+  </si>
+  <si>
+    <t>flower trig enables</t>
+  </si>
+  <si>
+    <t>LSB-&gt; pps trig enable, middle byte LSB-&gt; coinc trig enable, high byte LSB-&gt;ext trig enable</t>
   </si>
 </sst>
 </file>
@@ -816,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -903,6 +897,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -917,6 +912,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1199,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,38 +1211,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="A1" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="49">
+      <c r="A4" s="50">
         <v>44212</v>
       </c>
-      <c r="B4" s="50"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>37</v>
@@ -1419,7 +1415,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1955,7 +1951,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D41" s="43"/>
       <c r="E41" s="43"/>
@@ -2038,24 +2034,24 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="52">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B46" s="24" t="str">
+      <c r="B46" s="53" t="str">
         <f t="shared" si="0"/>
         <v>x27</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D46" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="E46" t="s">
-        <v>6</v>
-      </c>
-      <c r="F46" s="5" t="s">
+      <c r="E46" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="54" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2113,7 +2109,7 @@
         <v>29</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E49" t="s">
         <v>6</v>
@@ -2296,13 +2292,13 @@
         <v>21</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2318,13 +2314,13 @@
         <v>22</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2337,10 +2333,10 @@
         <v>x3A</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E65" s="34" t="s">
         <v>6</v>
@@ -2356,10 +2352,10 @@
         <v>x3B</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E66" s="34" t="s">
         <v>6</v>
@@ -2375,10 +2371,10 @@
         <v>x3C</v>
       </c>
       <c r="C67" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E67" s="34" t="s">
         <v>6</v>
@@ -2394,10 +2390,13 @@
         <v>x3D</v>
       </c>
       <c r="C68" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>170</v>
+        <v>198</v>
+      </c>
+      <c r="E68" s="46" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2409,14 +2408,10 @@
         <f t="shared" si="0"/>
         <v>x3E</v>
       </c>
-      <c r="C69" s="30" t="s">
-        <v>168</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>170</v>
-      </c>
+      <c r="C69" s="30"/>
+      <c r="D69" s="5"/>
       <c r="F69" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2428,12 +2423,8 @@
         <f t="shared" si="0"/>
         <v>x3F</v>
       </c>
-      <c r="C70" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>170</v>
-      </c>
+      <c r="C70" s="30"/>
+      <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
@@ -2483,10 +2474,10 @@
         <v>x42</v>
       </c>
       <c r="C73" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2647,10 +2638,10 @@
         <v>35</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E83" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2666,7 +2657,7 @@
         <v>106</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E84" t="s">
         <v>7</v>
@@ -2719,16 +2710,16 @@
         <f t="shared" si="2"/>
         <v>x50</v>
       </c>
-      <c r="C87" s="46" t="s">
+      <c r="C87" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="D87" s="47" t="s">
+      <c r="D87" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="E87" s="46" t="s">
+      <c r="E87" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="F87" s="47" t="s">
+      <c r="F87" s="48" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2741,16 +2732,16 @@
         <f t="shared" si="2"/>
         <v>x51</v>
       </c>
-      <c r="C88" s="46" t="s">
+      <c r="C88" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D88" s="47" t="s">
+      <c r="D88" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="E88" s="46" t="s">
+      <c r="E88" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="F88" s="47" t="s">
+      <c r="F88" s="48" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2763,16 +2754,16 @@
         <f t="shared" si="2"/>
         <v>x52</v>
       </c>
-      <c r="C89" s="46" t="s">
+      <c r="C89" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="D89" s="47" t="s">
+      <c r="D89" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="E89" s="46" t="s">
+      <c r="E89" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="F89" s="47" t="s">
+      <c r="F89" s="48" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2785,16 +2776,16 @@
         <f t="shared" si="2"/>
         <v>x53</v>
       </c>
-      <c r="C90" s="46" t="s">
+      <c r="C90" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="D90" s="47" t="s">
+      <c r="D90" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="E90" s="46" t="s">
+      <c r="E90" s="47" t="s">
         <v>166</v>
       </c>
-      <c r="F90" s="47" t="s">
+      <c r="F90" s="48" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2807,16 +2798,16 @@
         <f t="shared" si="2"/>
         <v>x54</v>
       </c>
-      <c r="C91" s="46" t="s">
+      <c r="C91" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="D91" s="46" t="s">
+      <c r="D91" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="E91" s="46" t="s">
+      <c r="E91" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F91" s="47" t="s">
+      <c r="F91" s="48" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2829,16 +2820,16 @@
         <f t="shared" si="2"/>
         <v>x55</v>
       </c>
-      <c r="C92" s="46" t="s">
+      <c r="C92" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="D92" s="47" t="s">
+      <c r="D92" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="E92" s="46" t="s">
+      <c r="E92" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F92" s="47"/>
+      <c r="F92" s="48"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
@@ -2861,10 +2852,10 @@
         <v>x57</v>
       </c>
       <c r="C94" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D94" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="D94" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="E94" s="45" t="s">
         <v>7</v>
@@ -2880,10 +2871,10 @@
         <v>x58</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E95" s="45" t="s">
         <v>7</v>
@@ -2899,10 +2890,10 @@
         <v>x59</v>
       </c>
       <c r="C96" s="45" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E96" s="45" t="s">
         <v>7</v>
@@ -2918,10 +2909,10 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="45" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E97" s="45" t="s">
         <v>7</v>
@@ -2937,13 +2928,13 @@
         <v>x5B</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E98" s="45" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3111,7 +3102,7 @@
         <v>144</v>
       </c>
       <c r="F110" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="111" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3127,7 +3118,7 @@
         <v>141</v>
       </c>
       <c r="F111" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="112" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3143,7 +3134,7 @@
         <v>142</v>
       </c>
       <c r="F112" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="113" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3159,7 +3150,7 @@
         <v>145</v>
       </c>
       <c r="F113" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3175,7 +3166,7 @@
         <v>146</v>
       </c>
       <c r="F114" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3238,7 +3229,7 @@
         <v>127</v>
       </c>
       <c r="F117" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="118" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3257,7 +3248,7 @@
         <v>125</v>
       </c>
       <c r="F118" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="119" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3276,7 +3267,7 @@
         <v>126</v>
       </c>
       <c r="F119" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="120" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3295,7 +3286,7 @@
         <v>126</v>
       </c>
       <c r="F120" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="121" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3314,7 +3305,7 @@
         <v>135</v>
       </c>
       <c r="F121" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="122" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3333,7 +3324,7 @@
         <v>126</v>
       </c>
       <c r="F122" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="123" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3352,7 +3343,7 @@
         <v>126</v>
       </c>
       <c r="F123" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="124" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3371,7 +3362,7 @@
         <v>137</v>
       </c>
       <c r="F124" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="125" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3390,7 +3381,7 @@
         <v>126</v>
       </c>
       <c r="F125" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="126" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3409,7 +3400,7 @@
         <v>126</v>
       </c>
       <c r="F126" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="127" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3425,7 +3416,7 @@
         <v>147</v>
       </c>
       <c r="F127" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="128" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3444,7 +3435,7 @@
         <v>143</v>
       </c>
       <c r="F128" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3467,10 +3458,10 @@
         <v>x7B</v>
       </c>
       <c r="C130" s="38" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F130" s="40" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="131" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -3483,10 +3474,10 @@
         <v>x7C</v>
       </c>
       <c r="C131" s="38" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F131" s="40" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -3521,21 +3512,21 @@
       </c>
     </row>
     <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A134" s="51">
+      <c r="A134" s="52">
         <f t="shared" si="3"/>
         <v>127</v>
       </c>
-      <c r="B134" s="52" t="str">
+      <c r="B134" s="53" t="str">
         <f t="shared" si="2"/>
         <v>x7F</v>
       </c>
-      <c r="C134" s="51" t="s">
+      <c r="C134" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="D134" s="53" t="s">
+      <c r="D134" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="E134" s="51" t="s">
+      <c r="E134" s="52" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
start updating register map
</commit_message>
<xml_diff>
--- a/doc/flower-register-map.xlsx
+++ b/doc/flower-register-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\projects\FLOWER-board-firmware\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CDD5B5-5C83-4ADA-8082-646D5C6BD07B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A35A680-E8BD-45FF-9C2A-C8DD4F8C1AF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2205" windowWidth="23235" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-570" yWindow="330" windowWidth="23235" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1195,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
featureful update to 0.6V firmware
increase pre-trig, add latched timestamp readout, config write RAM max address, update doc
</commit_message>
<xml_diff>
--- a/doc/flower-register-map.xlsx
+++ b/doc/flower-register-map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\projects\FLOWER-board-firmware\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAA6F46-C760-42FD-82A0-5BBD97F14FFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEF885A-9350-42BA-9D6C-5972230BA0B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="885" yWindow="300" windowWidth="23235" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="182">
   <si>
     <t>Register Map</t>
   </si>
@@ -168,9 +168,6 @@
     <t>pick scaler to read</t>
   </si>
   <si>
-    <t>currently 16 scalers registers (12 bits per scaler, 2 scalers per 24 bit register)</t>
-  </si>
-  <si>
     <t>write something between 0x0 and 0xF, scaler to read pops up in read-register 3</t>
   </si>
   <si>
@@ -186,36 +183,9 @@
     <t>reset event counter/timestamp</t>
   </si>
   <si>
-    <t>metadata-&gt;event counter low</t>
-  </si>
-  <si>
-    <t>metadata-&gt;event counter high</t>
-  </si>
-  <si>
-    <t>metadata-&gt;trig counter low</t>
-  </si>
-  <si>
-    <t>metadata-&gt;trig counter high</t>
-  </si>
-  <si>
-    <t>metadata-&gt;trig timestamp low</t>
-  </si>
-  <si>
-    <t>metadata-&gt;trig timestamp high</t>
-  </si>
-  <si>
-    <t>metadata-&gt;deadtime counter</t>
-  </si>
-  <si>
     <t>note: metadata assigned to these registers once event buffer set in register 78</t>
   </si>
   <si>
-    <t>metadata-&gt;(channel, beam masks)</t>
-  </si>
-  <si>
-    <t>metadata-&gt;unassigned</t>
-  </si>
-  <si>
     <t>bit0-&gt;global reset, bit1-&gt;reset global EXCEPT register settings, bit2-&gt;reset ADC (restart+cal cycle)</t>
   </si>
   <si>
@@ -228,57 +198,9 @@
     <t>chip ID is 64 bits: lower 24 bits</t>
   </si>
   <si>
-    <t>metadata-&gt;(buffer, cal_pulse_enabletrig_type, trig_lastbeam)</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 0</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 1</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 5</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 6</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 7</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 8</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 9</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 3</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 2</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 4</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 10</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 11</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 12</t>
-  </si>
-  <si>
-    <t>metadata-&gt;power beam 13</t>
-  </si>
-  <si>
     <t>set to: 0=1st buffer, 1=second,2=third,3=fourth</t>
   </si>
   <si>
-    <t>bits 23-22 : event buffer ; bit 21 : cal pulse switch ; bits 19-17 : pretrig window ; bits 16-15: trig type [0=nothing,1=software,2=phased trig,3=external] ; bits 14-0: last beam trigger</t>
-  </si>
-  <si>
     <t xml:space="preserve"> pick channel RAM to read out (i.e. 0x01 reads channel 0, reg value of 0 does nothing)</t>
   </si>
   <si>
@@ -318,9 +240,6 @@
     <t>clear readout process (might be helpful if hanging)</t>
   </si>
   <si>
-    <t>bits 3 to 0 -&gt; 1 indicates each ADCs locked datastream ; bits 11 to 8-&gt;ADC pd ; bit 16-&gt; adc startup signal</t>
-  </si>
-  <si>
     <t>NO FUNCTION</t>
   </si>
   <si>
@@ -351,9 +270,6 @@
     <t>default: phased trigger disabled at startup (LSB)</t>
   </si>
   <si>
-    <t>deadtime counter (num 25 MHz clk cycles) refreshed every second</t>
-  </si>
-  <si>
     <t>rdout-&gt;clear  buffer full, set buffer num to zero</t>
   </si>
   <si>
@@ -525,9 +441,6 @@
     <t>update register by writing LSB in reg 40</t>
   </si>
   <si>
-    <t>bit 23 : gate flag ; bits 22-15 : channel mask ; bits 14-0 : beam mask</t>
-  </si>
-  <si>
     <t>bit 0-&gt;enable; bit1-&gt;polarity; bit2-&gt; replace trigger output with 1Hz heartbeat pulse (debug use only) ; bits 8 to 15-&gt;width as specified by *93* MHz clock cycles</t>
   </si>
   <si>
@@ -540,15 +453,6 @@
     <t>note channel 5 hard-coded masked from trigger (dead vpol channel)</t>
   </si>
   <si>
-    <t>lower four bits clear each of the 4 event buffers, bit 8 sets buffer to 0, bit 16 is buffer clear for surface event buffer</t>
-  </si>
-  <si>
-    <t>x000404</t>
-  </si>
-  <si>
-    <t>bits 3 to 0-&gt;buffer full flags; bit 4-&gt;surface buffer full (slave board only); bit 8-&gt;OR of buffer full flags; bits 13 to 12-&gt;next_buffer ; bits 17 to 16-&gt; last trig type</t>
-  </si>
-  <si>
     <t>FLOWER board</t>
   </si>
   <si>
@@ -624,20 +528,65 @@
     <t>lowest byte : num_coinc (0 = 1 ch); middle byte : coinc_window; high byte (LSB = 1 vpp mode; =0 single-side Vp mode)</t>
   </si>
   <si>
-    <t>lower three bits used, set value to 0 thru 7.</t>
-  </si>
-  <si>
     <t>flower trig enables</t>
   </si>
   <si>
     <t>LSB-&gt; pps trig enable, middle byte LSB-&gt; coinc trig enable, high byte LSB-&gt;ext trig enable</t>
+  </si>
+  <si>
+    <t>LSB</t>
+  </si>
+  <si>
+    <t>read_only -- bit 0 = buffer_full, bit 8 = write_busy</t>
+  </si>
+  <si>
+    <t>x0003FF</t>
+  </si>
+  <si>
+    <t>write-&gt;ram depth (event length)</t>
+  </si>
+  <si>
+    <t>don't touch after board setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">event metadata-&gt;event counter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">event metadata-&gt;trig counter </t>
+  </si>
+  <si>
+    <t>event metadata-&gt;trig timestamp low</t>
+  </si>
+  <si>
+    <t>event metadata-&gt;trig timestamp high</t>
+  </si>
+  <si>
+    <t>event metadata-&gt;info</t>
+  </si>
+  <si>
+    <t>read_only - event meta data [lowest 4 bits=trigger type, bit16=pps flag]</t>
+  </si>
+  <si>
+    <t>currently 32 scalers registers (12 bits per scaler, 2 scalers per 24 bit register)</t>
+  </si>
+  <si>
+    <t>data in max_address location may not be useful</t>
+  </si>
+  <si>
+    <t>x000004</t>
+  </si>
+  <si>
+    <t>max = 1023 (0x3FF), record length corresponds to 4 * value / sampling rate</t>
+  </si>
+  <si>
+    <t>lower four bits used, set value to 0 thru 8.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,6 +654,21 @@
     <font>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -810,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -902,9 +866,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -913,6 +874,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1195,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,38 +1182,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="A1" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="50">
+      <c r="A4" s="54">
         <v>44212</v>
       </c>
-      <c r="B4" s="51"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>37</v>
@@ -1262,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
@@ -1285,10 +1256,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="F7" s="13"/>
     </row>
@@ -1333,13 +1304,13 @@
         <v>x03</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1358,7 +1329,7 @@
         <v>36</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1390,16 +1361,16 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1412,29 +1383,23 @@
         <v>40</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B15" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>x08</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="56" t="s">
         <v>16</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B15" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>x08</v>
-      </c>
-      <c r="C15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1446,10 +1411,10 @@
         <f t="shared" si="0"/>
         <v>x09</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="C16" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="56" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1463,16 +1428,16 @@
         <v>x0A</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>50</v>
+        <v>171</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1485,10 +1450,10 @@
         <v>x0B</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>51</v>
+        <v>172</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>6</v>
@@ -1505,10 +1470,10 @@
         <v>x0C</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>6</v>
@@ -1525,10 +1490,10 @@
         <v>x0D</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>53</v>
+        <v>174</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>6</v>
@@ -1545,10 +1510,10 @@
         <v>x0E</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>54</v>
+        <v>175</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>6</v>
@@ -1564,15 +1529,6 @@
         <f t="shared" si="0"/>
         <v>x0F</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>6</v>
-      </c>
       <c r="F22" s="19"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1584,20 +1540,12 @@
         <f t="shared" si="0"/>
         <v>x10</v>
       </c>
-      <c r="C23" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1606,18 +1554,10 @@
         <f t="shared" si="0"/>
         <v>x11</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>80</v>
-      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
@@ -1628,18 +1568,10 @@
         <f t="shared" si="0"/>
         <v>x12</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>163</v>
-      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="19"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
@@ -1650,15 +1582,9 @@
         <f t="shared" si="0"/>
         <v>x13</v>
       </c>
-      <c r="C26" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="19"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1670,15 +1596,9 @@
         <f t="shared" si="0"/>
         <v>x14</v>
       </c>
-      <c r="C27" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1690,15 +1610,9 @@
         <f t="shared" si="0"/>
         <v>x15</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="19"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1710,15 +1624,9 @@
         <f t="shared" si="0"/>
         <v>x16</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="19"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1730,15 +1638,9 @@
         <f t="shared" si="0"/>
         <v>x17</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1750,15 +1652,9 @@
         <f t="shared" si="0"/>
         <v>x18</v>
       </c>
-      <c r="C31" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
       <c r="F31" s="19"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1770,15 +1666,9 @@
         <f t="shared" si="0"/>
         <v>x19</v>
       </c>
-      <c r="C32" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
       <c r="F32" s="19"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1790,15 +1680,9 @@
         <f t="shared" si="0"/>
         <v>x1A</v>
       </c>
-      <c r="C33" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
       <c r="F33" s="19"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1810,15 +1694,9 @@
         <f t="shared" si="0"/>
         <v>x1B</v>
       </c>
-      <c r="C34" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
       <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1830,15 +1708,9 @@
         <f t="shared" si="0"/>
         <v>x1C</v>
       </c>
-      <c r="C35" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
       <c r="F35" s="19"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1850,15 +1722,9 @@
         <f t="shared" si="0"/>
         <v>x1D</v>
       </c>
-      <c r="C36" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
       <c r="F36" s="19"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1870,15 +1736,9 @@
         <f t="shared" si="0"/>
         <v>x1E</v>
       </c>
-      <c r="C37" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
       <c r="F37" s="19"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1890,15 +1750,9 @@
         <f t="shared" si="0"/>
         <v>x1F</v>
       </c>
-      <c r="C38" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
       <c r="F38" s="19"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1910,15 +1764,9 @@
         <f t="shared" si="0"/>
         <v>x20</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
       <c r="F39" s="19"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1930,15 +1778,9 @@
         <f t="shared" si="0"/>
         <v>x21</v>
       </c>
-      <c r="C40" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
       <c r="F40" s="19"/>
     </row>
     <row r="41" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -1951,7 +1793,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="D41" s="43"/>
       <c r="E41" s="43"/>
@@ -1967,13 +1809,13 @@
         <v>x23</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1986,13 +1828,13 @@
         <v>x24</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2005,13 +1847,13 @@
         <v>x25</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2024,35 +1866,35 @@
         <v>x26</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="52">
+      <c r="A46" s="49">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B46" s="53" t="str">
+      <c r="B46" s="50" t="str">
         <f t="shared" si="0"/>
         <v>x27</v>
       </c>
-      <c r="C46" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D46" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="E46" s="52" t="s">
+      <c r="C46" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="F46" s="54" t="s">
-        <v>102</v>
+      <c r="F46" s="51" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2065,10 +1907,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="D47" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -2087,13 +1929,13 @@
         <v>43</v>
       </c>
       <c r="D48" t="s">
-        <v>44</v>
+        <v>177</v>
       </c>
       <c r="E48" t="s">
         <v>6</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2109,7 +1951,7 @@
         <v>29</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="E49" t="s">
         <v>6</v>
@@ -2138,13 +1980,13 @@
         <v>x2C</v>
       </c>
       <c r="C51" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="D51" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2157,13 +1999,13 @@
         <v>x2D</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2206,7 +2048,7 @@
         <v>42</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2292,13 +2134,13 @@
         <v>21</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2314,13 +2156,13 @@
         <v>22</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2333,10 +2175,10 @@
         <v>x3A</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
       <c r="E65" s="34" t="s">
         <v>6</v>
@@ -2352,10 +2194,10 @@
         <v>x3B</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>178</v>
+        <v>146</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="E66" s="34" t="s">
         <v>6</v>
@@ -2371,10 +2213,10 @@
         <v>x3C</v>
       </c>
       <c r="C67" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="E67" s="34" t="s">
         <v>6</v>
@@ -2390,10 +2232,10 @@
         <v>x3D</v>
       </c>
       <c r="C68" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>198</v>
+        <v>165</v>
       </c>
       <c r="E68" s="46" t="s">
         <v>6</v>
@@ -2411,7 +2253,7 @@
       <c r="C69" s="30"/>
       <c r="D69" s="5"/>
       <c r="F69" s="5" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2458,7 +2300,7 @@
         <v>10</v>
       </c>
       <c r="D72" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="E72" t="s">
         <v>7</v>
@@ -2474,10 +2316,13 @@
         <v>x42</v>
       </c>
       <c r="C73" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>184</v>
+        <v>152</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2500,7 +2345,18 @@
         <f t="shared" si="2"/>
         <v>x44</v>
       </c>
-      <c r="F75" s="10"/>
+      <c r="C75" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="F75" s="29" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
@@ -2515,13 +2371,13 @@
         <v>24</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="E76" t="s">
         <v>7</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2554,7 +2410,7 @@
         <v>7</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2576,7 +2432,7 @@
         <v>7</v>
       </c>
       <c r="F79" s="22" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2612,17 +2468,17 @@
         <f t="shared" si="2"/>
         <v>x4B</v>
       </c>
-      <c r="C82" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D82" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="F82" s="29" t="s">
-        <v>154</v>
+      <c r="C82" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="D82" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="E82" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="F82" s="58" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2638,13 +2494,13 @@
         <v>35</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="E83" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="3"/>
         <v>77</v>
@@ -2654,16 +2510,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E84" t="s">
         <v>7</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2675,17 +2531,17 @@
         <f t="shared" si="2"/>
         <v>x4E</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="F85" s="5" t="s">
-        <v>79</v>
+      <c r="F85" s="57" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2717,7 +2573,7 @@
         <v>34</v>
       </c>
       <c r="E87" s="47" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F87" s="48" t="s">
         <v>33</v>
@@ -2733,16 +2589,16 @@
         <v>x51</v>
       </c>
       <c r="C88" s="47" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D88" s="48" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="E88" s="47" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="F88" s="48" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2755,16 +2611,16 @@
         <v>x52</v>
       </c>
       <c r="C89" s="47" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="D89" s="48" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="E89" s="47" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="F89" s="48" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2777,16 +2633,16 @@
         <v>x53</v>
       </c>
       <c r="C90" s="47" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="D90" s="48" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="E90" s="47" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="F90" s="48" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2799,16 +2655,16 @@
         <v>x54</v>
       </c>
       <c r="C91" s="47" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="D91" s="47" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E91" s="47" t="s">
         <v>7</v>
       </c>
       <c r="F91" s="48" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2821,10 +2677,10 @@
         <v>x55</v>
       </c>
       <c r="C92" s="47" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="D92" s="48" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="E92" s="47" t="s">
         <v>11</v>
@@ -2852,10 +2708,10 @@
         <v>x57</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="E94" s="45" t="s">
         <v>7</v>
@@ -2871,10 +2727,10 @@
         <v>x58</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="E95" s="45" t="s">
         <v>7</v>
@@ -2890,10 +2746,10 @@
         <v>x59</v>
       </c>
       <c r="C96" s="45" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="E96" s="45" t="s">
         <v>7</v>
@@ -2909,10 +2765,10 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="45" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="E97" s="45" t="s">
         <v>7</v>
@@ -2928,13 +2784,13 @@
         <v>x5B</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="E98" s="45" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3077,13 +2933,13 @@
         <v>x66</v>
       </c>
       <c r="D109" s="35" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="E109" s="35" t="s">
         <v>6</v>
       </c>
       <c r="F109" s="37" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
     </row>
     <row r="110" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3096,13 +2952,13 @@
         <v>x67</v>
       </c>
       <c r="C110" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D110" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F110" s="33" t="s">
         <v>140</v>
-      </c>
-      <c r="D110" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="F110" s="33" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="111" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3115,10 +2971,10 @@
         <v>x68</v>
       </c>
       <c r="C111" s="31" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="F111" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="112" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3131,10 +2987,10 @@
         <v>x69</v>
       </c>
       <c r="C112" s="31" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="F112" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="113" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3147,10 +3003,10 @@
         <v>x6A</v>
       </c>
       <c r="C113" s="31" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="F113" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="114" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3163,10 +3019,10 @@
         <v>x6B</v>
       </c>
       <c r="C114" s="31" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F114" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3179,16 +3035,16 @@
         <v>x6C</v>
       </c>
       <c r="C115" s="27" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D115" s="27" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="E115" s="27" t="s">
         <v>6</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3201,7 +3057,7 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="D116" t="s">
         <v>18</v>
@@ -3210,7 +3066,7 @@
         <v>19</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="117" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3223,13 +3079,13 @@
         <v>x6E</v>
       </c>
       <c r="C117" s="31" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="D117" s="31" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="F117" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="118" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3242,13 +3098,13 @@
         <v>x6F</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="D118" s="31" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="F118" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="119" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3261,13 +3117,13 @@
         <v>x70</v>
       </c>
       <c r="C119" s="31" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="D119" s="31" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="F119" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="120" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3280,13 +3136,13 @@
         <v>x71</v>
       </c>
       <c r="C120" s="31" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="D120" s="31" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="F120" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="121" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3299,13 +3155,13 @@
         <v>x72</v>
       </c>
       <c r="C121" s="31" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="D121" s="31" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="F121" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="122" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3318,13 +3174,13 @@
         <v>x73</v>
       </c>
       <c r="C122" s="31" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="D122" s="31" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="F122" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3337,13 +3193,13 @@
         <v>x74</v>
       </c>
       <c r="C123" s="31" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="D123" s="31" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="F123" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="124" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3356,13 +3212,13 @@
         <v>x75</v>
       </c>
       <c r="C124" s="31" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="D124" s="31" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="F124" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="125" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3375,13 +3231,13 @@
         <v>x76</v>
       </c>
       <c r="C125" s="31" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="D125" s="31" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="F125" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="126" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3394,13 +3250,13 @@
         <v>x77</v>
       </c>
       <c r="C126" s="31" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="D126" s="31" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="F126" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="127" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3413,10 +3269,10 @@
         <v>x78</v>
       </c>
       <c r="C127" s="31" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="F127" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="128" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3429,13 +3285,13 @@
         <v>x79</v>
       </c>
       <c r="C128" s="31" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="D128" s="31" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="F128" s="33" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3458,10 +3314,10 @@
         <v>x7B</v>
       </c>
       <c r="C130" s="38" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
       <c r="F130" s="40" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
     </row>
     <row r="131" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
@@ -3474,10 +3330,10 @@
         <v>x7C</v>
       </c>
       <c r="C131" s="38" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="F131" s="40" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -3502,31 +3358,31 @@
         <v>x7E</v>
       </c>
       <c r="C133" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D133" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E133" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A134" s="52">
+      <c r="A134" s="49">
         <f t="shared" si="3"/>
         <v>127</v>
       </c>
-      <c r="B134" s="53" t="str">
+      <c r="B134" s="50" t="str">
         <f t="shared" si="2"/>
         <v>x7F</v>
       </c>
-      <c r="C134" s="52" t="s">
+      <c r="C134" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D134" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="E134" s="52" t="s">
+      <c r="D134" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="E134" s="49" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add pps_delay to sys_trig_out
Add option for sending delayed PPS signal as a trigger output to the RADIANT, most useful for pulser time sweeps
</commit_message>
<xml_diff>
--- a/doc/flower-register-map.xlsx
+++ b/doc/flower-register-map.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\projects\FLOWER-board-firmware\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erico\Desktop\projects\greenland_lowthreshold_system\FLOWER-board-firmware\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B9F9CC-4F3C-4C5D-8A09-FC143765EB92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="600" windowWidth="23235" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1455" yWindow="600" windowWidth="23235" windowHeight="14700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="190">
   <si>
     <t>Register Map</t>
   </si>
@@ -582,9 +581,6 @@
     <t>reset board via power cycle</t>
   </si>
   <si>
-    <t>LSB = coinc trig to sys_trig_out</t>
-  </si>
-  <si>
     <t>SYSTEM TRIGGER CONFIG-&gt; send to system trigger output</t>
   </si>
   <si>
@@ -598,12 +594,21 @@
   </si>
   <si>
     <t>Approx 68ns pre-trigger per chunk</t>
+  </si>
+  <si>
+    <t>PPS trigger delay</t>
+  </si>
+  <si>
+    <t>10MHz clk increment delay, 24 bits</t>
+  </si>
+  <si>
+    <t>low-byte LSB sends  coinc trig to sys_trig_out; middle byte LSB sends delayed pps to sys_trig_out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -793,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -901,6 +906,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1183,11 +1189,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B62" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,38 +1208,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="58">
+      <c r="A4" s="59">
         <v>44212</v>
       </c>
-      <c r="B4" s="59"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>37</v>
@@ -2514,13 +2520,13 @@
         <v>35</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E83" t="s">
         <v>179</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2816,7 +2822,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="3"/>
         <v>92</v>
@@ -2826,10 +2832,10 @@
         <v>x5C</v>
       </c>
       <c r="C99" s="49" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="E99" s="49" t="s">
         <v>11</v>
@@ -2845,10 +2851,10 @@
         <v>x5D</v>
       </c>
       <c r="C100" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D100" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="E100" s="49" t="s">
         <v>7</v>
@@ -2863,9 +2869,15 @@
         <f t="shared" si="2"/>
         <v>x5E</v>
       </c>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
+      <c r="C101" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E101" s="57" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">

</xml_diff>